<commit_message>
BUG FIX on placing nerve in cuff and maintaining thk_medium_gap_internal!
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Sample</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Model Index</t>
   </si>
   <si>
-    <t>polyfasc</t>
-  </si>
-  <si>
     <t>Purdue</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Model 1</t>
   </si>
   <si>
-    <t>CorTec 200</t>
-  </si>
-  <si>
     <t>Model 2</t>
   </si>
   <si>
@@ -121,6 +115,9 @@
   </si>
   <si>
     <t>cuff too small</t>
+  </si>
+  <si>
+    <t>CorTec 300</t>
   </si>
 </sst>
 </file>
@@ -491,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,16 +506,16 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -539,7 +536,7 @@
       </c>
       <c r="C4" s="7"/>
       <c r="F4" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -621,8 +618,9 @@
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>22</v>
+      <c r="C15" s="7"/>
+      <c r="F15" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,7 +686,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
       <c r="F21" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -722,9 +720,6 @@
       <c r="B24" s="4">
         <v>17</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -741,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -762,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixes for EP from multi models in a single run
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="82">
   <si>
     <t>Sample</t>
   </si>
@@ -132,6 +132,144 @@
   </si>
   <si>
     <t>MicroLeads300</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Cervical</t>
+  </si>
+  <si>
+    <t>Abdominal</t>
+  </si>
+  <si>
+    <t>Cadaver</t>
+  </si>
+  <si>
+    <t>54-3</t>
+  </si>
+  <si>
+    <t>55-3</t>
+  </si>
+  <si>
+    <t>57-3</t>
+  </si>
+  <si>
+    <t>53-2</t>
+  </si>
+  <si>
+    <t>50-2</t>
+  </si>
+  <si>
+    <t>47-2</t>
+  </si>
+  <si>
+    <t>58-3</t>
+  </si>
+  <si>
+    <t>56-3</t>
+  </si>
+  <si>
+    <t>46-2</t>
+  </si>
+  <si>
+    <t>70-1</t>
+  </si>
+  <si>
+    <t>69-1</t>
+  </si>
+  <si>
+    <t>64-1</t>
+  </si>
+  <si>
+    <t>57-1</t>
+  </si>
+  <si>
+    <t>54-2</t>
+  </si>
+  <si>
+    <t>63-1</t>
+  </si>
+  <si>
+    <t>56-1</t>
+  </si>
+  <si>
+    <t>65-1</t>
+  </si>
+  <si>
+    <t>58-1</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>13-1</t>
+  </si>
+  <si>
+    <t>11-1</t>
+  </si>
+  <si>
+    <t>12-1</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>5-1</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>8-7</t>
+  </si>
+  <si>
+    <t>9-3</t>
+  </si>
+  <si>
+    <t>14-2</t>
+  </si>
+  <si>
+    <t>15-2</t>
+  </si>
+  <si>
+    <t>13-3</t>
+  </si>
+  <si>
+    <t>11-3</t>
+  </si>
+  <si>
+    <t>12-3</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>5-3</t>
+  </si>
+  <si>
+    <t>8-1</t>
+  </si>
+  <si>
+    <t>10-1</t>
+  </si>
+  <si>
+    <t>14-3</t>
+  </si>
+  <si>
+    <t>15-3</t>
   </si>
 </sst>
 </file>
@@ -191,18 +329,9 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -212,22 +341,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,416 +636,1180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G32"/>
+  <dimension ref="A2:R73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:E24"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="D5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="H5"/>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="D10">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="D11">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6">
+      <c r="D14" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="E14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="G14" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B16">
+      <c r="D15">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="E15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B17">
+      <c r="D16">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B18">
+      <c r="D17">
         <v>12</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="E17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19">
+      <c r="D18">
         <v>13</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="C20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="E19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B21">
+      <c r="D20">
         <v>14</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="E20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B22">
+      <c r="D21">
         <v>15</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="E21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B23">
+      <c r="D22">
         <v>16</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="E22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="G22" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="6">
+      <c r="D23" s="4">
         <v>17</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="E23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="G23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25">
+        <v>18</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
       </c>
       <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29">
+        <v>22</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31">
+        <v>23</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32">
+        <v>24</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33">
+        <v>25</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>26</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36">
+        <v>27</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39">
         <v>30</v>
       </c>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40">
+        <v>31</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42">
+        <v>32</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43">
+        <v>33</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44">
+        <v>34</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45">
+        <v>35</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47">
+        <v>36</v>
+      </c>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48">
+        <v>37</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49">
+        <v>38</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51">
+        <v>39</v>
+      </c>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52">
+        <v>40</v>
+      </c>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53">
+        <v>41</v>
+      </c>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54">
+        <v>42</v>
+      </c>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55">
+        <v>43</v>
+      </c>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56">
+        <v>44</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57">
+        <v>45</v>
+      </c>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58">
+        <v>46</v>
+      </c>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59">
+        <v>47</v>
+      </c>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61">
+        <v>48</v>
+      </c>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62">
+        <v>49</v>
+      </c>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63">
+        <v>50</v>
+      </c>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65">
+        <v>51</v>
+      </c>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66">
+        <v>52</v>
+      </c>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67">
+        <v>53</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68">
+        <v>54</v>
+      </c>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69">
+        <v>55</v>
+      </c>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D70">
+        <v>56</v>
+      </c>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71">
+        <v>57</v>
+      </c>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72">
+        <v>58</v>
+      </c>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D73">
+        <v>59</v>
+      </c>
+      <c r="E73" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds CorTec 400, bug fix in TubeCuff when tiny gap.
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="83">
   <si>
     <t>Sample</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>15-3</t>
+  </si>
+  <si>
+    <t>use 400</t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,6 +709,9 @@
       <c r="G3" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="L3" t="s">
+        <v>82</v>
+      </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
       </c>
@@ -732,6 +738,9 @@
       <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L4" t="s">
+        <v>82</v>
+      </c>
       <c r="O4">
         <v>0</v>
       </c>
@@ -762,6 +771,9 @@
         <v>34</v>
       </c>
       <c r="H5"/>
+      <c r="L5" t="s">
+        <v>82</v>
+      </c>
       <c r="O5">
         <v>1</v>
       </c>
@@ -793,6 +805,9 @@
       <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L6" t="s">
+        <v>82</v>
+      </c>
       <c r="O6">
         <v>2</v>
       </c>
@@ -821,6 +836,9 @@
       </c>
       <c r="G7" s="3" t="s">
         <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>82</v>
       </c>
       <c r="O7">
         <v>3</v>
@@ -863,6 +881,9 @@
       <c r="G9" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -886,6 +907,9 @@
       <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L10" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -909,6 +933,9 @@
       <c r="G11" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -932,6 +959,9 @@
       <c r="G12" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
@@ -959,6 +989,7 @@
       <c r="G14" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="L14"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1006,7 +1037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1029,7 +1060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1052,13 +1083,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
       <c r="C19" s="12"/>
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1081,7 +1112,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1104,7 +1135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1127,7 +1158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1149,8 +1180,9 @@
       <c r="G23" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L23"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1166,7 +1198,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1182,7 +1214,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1199,7 +1231,7 @@
       <c r="F27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1215,7 +1247,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1231,10 +1263,10 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1250,7 +1282,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
lots of lots of mnr
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -272,14 +272,14 @@
     <t>15-3</t>
   </si>
   <si>
-    <t>use 400</t>
+    <t>CorTec400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +289,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -344,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -359,6 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,7 +650,7 @@
   <dimension ref="A2:R73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,8 +659,10 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -700,16 +710,16 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
+      <c r="H3" s="3" t="s">
         <v>82</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -738,7 +748,7 @@
       <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L4" t="s">
+      <c r="H4" s="3" t="s">
         <v>82</v>
       </c>
       <c r="O4">
@@ -770,10 +780,10 @@
       <c r="G5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H5"/>
-      <c r="L5" t="s">
+      <c r="H5" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="L5"/>
       <c r="O5">
         <v>1</v>
       </c>
@@ -805,7 +815,7 @@
       <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L6" t="s">
+      <c r="H6" s="3" t="s">
         <v>82</v>
       </c>
       <c r="O6">
@@ -837,7 +847,7 @@
       <c r="G7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L7" t="s">
+      <c r="H7" s="3" t="s">
         <v>82</v>
       </c>
       <c r="O7">
@@ -857,6 +867,7 @@
       <c r="C8" s="12"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
+      <c r="H8" s="14"/>
       <c r="O8">
         <v>4</v>
       </c>
@@ -881,7 +892,7 @@
       <c r="G9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L9" t="s">
+      <c r="H9" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -907,7 +918,7 @@
       <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L10" t="s">
+      <c r="H10" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -933,7 +944,7 @@
       <c r="G11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
+      <c r="H11" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -959,7 +970,7 @@
       <c r="G12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L12" t="s">
+      <c r="H12" s="3" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds parameters for shape and solution order to model in "solution" Object: node, by default, we want shape_order = 2, and sorder = "quadratic"
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="88">
   <si>
     <t>Sample</t>
   </si>
@@ -273,6 +273,21 @@
   </si>
   <si>
     <t>191205-0</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>2019 Segmentation</t>
+  </si>
+  <si>
+    <t>20% Shrink</t>
+  </si>
+  <si>
+    <t>0% Shrink</t>
+  </si>
+  <si>
+    <t>2020 Segmentation</t>
   </si>
 </sst>
 </file>
@@ -301,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -333,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -351,6 +372,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,28 +666,29 @@
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="F1" s="14" t="s">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="14"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="J1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="14"/>
       <c r="M1" s="14"/>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>30</v>
       </c>
@@ -674,680 +698,739 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P5"/>
       <c r="Q5"/>
       <c r="R5"/>
       <c r="S5"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>33</v>
-      </c>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="10"/>
       <c r="D8" s="9"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="11"/>
-      <c r="K8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="11"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="10"/>
-      <c r="D9" s="9" t="s">
+      <c r="M8" s="3"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11">
         <v>7</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12">
         <v>8</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="3">
         <v>9</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15">
         <v>10</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16">
         <v>11</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17">
         <v>12</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18">
         <v>13</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J18" s="3"/>
       <c r="L18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N18" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="D19" s="9"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="4"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20">
         <v>14</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21">
         <v>15</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22">
         <v>16</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="3">
         <v>17</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G23" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -1357,13 +1440,14 @@
       <c r="D25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1"/>
+      <c r="F25">
         <v>18</v>
       </c>
-      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>35</v>
       </c>
@@ -1373,13 +1457,14 @@
       <c r="D26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1"/>
+      <c r="F26">
         <v>19</v>
       </c>
-      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -1389,14 +1474,15 @@
       <c r="D27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E27">
-        <v>20</v>
-      </c>
-      <c r="F27" s="3"/>
+      <c r="E27" s="1"/>
+      <c r="F27">
+        <v>20</v>
+      </c>
       <c r="G27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>35</v>
       </c>
@@ -1406,13 +1492,14 @@
       <c r="D28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1"/>
+      <c r="F28">
         <v>21</v>
       </c>
-      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -1422,16 +1509,17 @@
       <c r="D29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1"/>
+      <c r="F29">
         <v>22</v>
       </c>
-      <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>35</v>
       </c>
@@ -1441,13 +1529,13 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>23</v>
       </c>
-      <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>35</v>
       </c>
@@ -1457,13 +1545,13 @@
       <c r="D32" t="s">
         <v>42</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>24</v>
       </c>
-      <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>35</v>
       </c>
@@ -1473,13 +1561,13 @@
       <c r="D33" t="s">
         <v>43</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>25</v>
       </c>
-      <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>35</v>
       </c>
@@ -1489,16 +1577,16 @@
       <c r="D34" t="s">
         <v>44</v>
       </c>
-      <c r="E34">
-        <v>26</v>
-      </c>
-      <c r="F34" s="3"/>
+      <c r="F34">
+        <v>26</v>
+      </c>
       <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -1508,12 +1596,12 @@
       <c r="D36" t="s">
         <v>45</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>27</v>
       </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -1523,12 +1611,12 @@
       <c r="D37" t="s">
         <v>46</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>28</v>
       </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>35</v>
       </c>
@@ -1538,12 +1626,12 @@
       <c r="D38" t="s">
         <v>47</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>29</v>
       </c>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>35</v>
       </c>
@@ -1553,12 +1641,12 @@
       <c r="D39" t="s">
         <v>48</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>30</v>
       </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>35</v>
       </c>
@@ -1568,15 +1656,15 @@
       <c r="D40" t="s">
         <v>49</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>31</v>
       </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>35</v>
       </c>
@@ -1586,12 +1674,12 @@
       <c r="D42" t="s">
         <v>50</v>
       </c>
-      <c r="E42">
-        <v>32</v>
-      </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>32</v>
+      </c>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>35</v>
       </c>
@@ -1601,12 +1689,12 @@
       <c r="D43" t="s">
         <v>51</v>
       </c>
-      <c r="E43">
-        <v>33</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>33</v>
+      </c>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>35</v>
       </c>
@@ -1616,12 +1704,12 @@
       <c r="D44" t="s">
         <v>52</v>
       </c>
-      <c r="E44">
-        <v>34</v>
-      </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>34</v>
+      </c>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>35</v>
       </c>
@@ -1631,15 +1719,15 @@
       <c r="D45" t="s">
         <v>53</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>35</v>
       </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>54</v>
       </c>
@@ -1649,12 +1737,12 @@
       <c r="D47" t="s">
         <v>55</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>36</v>
       </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>54</v>
       </c>
@@ -1664,12 +1752,13 @@
       <c r="D48" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="12"/>
+      <c r="F48">
         <v>37</v>
       </c>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>54</v>
       </c>
@@ -1679,15 +1768,16 @@
       <c r="D49" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="16"/>
+      <c r="F49">
         <v>38</v>
       </c>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>54</v>
       </c>
@@ -1697,12 +1787,13 @@
       <c r="D51" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="16"/>
+      <c r="F51">
         <v>39</v>
       </c>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>54</v>
       </c>
@@ -1712,12 +1803,13 @@
       <c r="D52" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="16"/>
+      <c r="F52">
         <v>40</v>
       </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>54</v>
       </c>
@@ -1727,12 +1819,13 @@
       <c r="D53" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="16"/>
+      <c r="F53">
         <v>41</v>
       </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>54</v>
       </c>
@@ -1742,12 +1835,13 @@
       <c r="D54" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="16"/>
+      <c r="F54">
         <v>42</v>
       </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -1757,12 +1851,13 @@
       <c r="D55" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="16"/>
+      <c r="F55">
         <v>43</v>
       </c>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>54</v>
       </c>
@@ -1772,12 +1867,13 @@
       <c r="D56" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="16"/>
+      <c r="F56">
         <v>44</v>
       </c>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>54</v>
       </c>
@@ -1787,12 +1883,13 @@
       <c r="D57" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="16"/>
+      <c r="F57">
         <v>45</v>
       </c>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>54</v>
       </c>
@@ -1802,12 +1899,13 @@
       <c r="D58" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="16"/>
+      <c r="F58">
         <v>46</v>
       </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>54</v>
       </c>
@@ -1817,15 +1915,16 @@
       <c r="D59" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="16"/>
+      <c r="F59">
         <v>47</v>
       </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>54</v>
       </c>
@@ -1835,12 +1934,12 @@
       <c r="D61" t="s">
         <v>67</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>48</v>
       </c>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>54</v>
       </c>
@@ -1850,12 +1949,13 @@
       <c r="D62" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="12"/>
+      <c r="F62">
         <v>49</v>
       </c>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>54</v>
       </c>
@@ -1865,15 +1965,16 @@
       <c r="D63" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="12"/>
+      <c r="F63">
         <v>50</v>
       </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>54</v>
       </c>
@@ -1883,12 +1984,13 @@
       <c r="D65" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="16"/>
+      <c r="F65">
         <v>51</v>
       </c>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>54</v>
       </c>
@@ -1898,12 +2000,13 @@
       <c r="D66" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="16"/>
+      <c r="F66">
         <v>52</v>
       </c>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>54</v>
       </c>
@@ -1913,12 +2016,13 @@
       <c r="D67" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="16"/>
+      <c r="F67">
         <v>53</v>
       </c>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>54</v>
       </c>
@@ -1928,12 +2032,13 @@
       <c r="D68" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E68">
-        <v>54</v>
-      </c>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E68" s="16"/>
+      <c r="F68">
+        <v>54</v>
+      </c>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>54</v>
       </c>
@@ -1943,12 +2048,13 @@
       <c r="D69" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="16"/>
+      <c r="F69">
         <v>55</v>
       </c>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>54</v>
       </c>
@@ -1958,12 +2064,13 @@
       <c r="D70" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="16"/>
+      <c r="F70">
         <v>56</v>
       </c>
-      <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>54</v>
       </c>
@@ -1973,12 +2080,13 @@
       <c r="D71" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="16"/>
+      <c r="F71">
         <v>57</v>
       </c>
-      <c r="F71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>54</v>
       </c>
@@ -1988,12 +2096,13 @@
       <c r="D72" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="16"/>
+      <c r="F72">
         <v>58</v>
       </c>
-      <c r="F72" s="3"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>54</v>
       </c>
@@ -2003,12 +2112,13 @@
       <c r="D73" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="16"/>
+      <c r="F73">
         <v>59</v>
       </c>
-      <c r="F73" s="3"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="3"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2021,14 +2131,412 @@
       <c r="D75" t="s">
         <v>82</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F75">
         <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F76">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>500</v>
+      </c>
+      <c r="B78" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F78">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>100</v>
+      </c>
+      <c r="B79" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F79">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>100</v>
+      </c>
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F80" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>100</v>
+      </c>
+      <c r="B81" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F81">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>100</v>
+      </c>
+      <c r="B82" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F82">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C83" s="10"/>
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>100</v>
+      </c>
+      <c r="B84" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F84">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>100</v>
+      </c>
+      <c r="B85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F85">
+        <v>68</v>
+      </c>
+      <c r="I85" s="3"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>100</v>
+      </c>
+      <c r="B86" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F86">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>100</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F87">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C88" s="10"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F89" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>100</v>
+      </c>
+      <c r="B90" t="s">
+        <v>32</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F90">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>100</v>
+      </c>
+      <c r="B91" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F91">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>100</v>
+      </c>
+      <c r="B92" t="s">
+        <v>32</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E92" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F92">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>100</v>
+      </c>
+      <c r="B93" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E93" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F93">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C94" s="10"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>100</v>
+      </c>
+      <c r="B95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F95">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>10</v>
+      </c>
+      <c r="B96" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F96">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>100</v>
+      </c>
+      <c r="B97" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F97">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>100</v>
+      </c>
+      <c r="B98" t="s">
+        <v>32</v>
+      </c>
+      <c r="C98" t="s">
+        <v>34</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F98" s="3">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cuff pos bug fix!
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="94">
   <si>
     <t>Sample</t>
   </si>
@@ -291,6 +291,21 @@
   </si>
   <si>
     <t>Purdue cuff not fitting properly</t>
+  </si>
+  <si>
+    <t>nerve messed up</t>
+  </si>
+  <si>
+    <t>Purdue - nerve int elec</t>
+  </si>
+  <si>
+    <t>CorTec - nerve extending out of fill in same spot as purdue</t>
+  </si>
+  <si>
+    <t>MicroLeads 500 is good</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CorTec 400 same issue</t>
   </si>
 </sst>
 </file>
@@ -363,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -383,7 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92:K98"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +2001,7 @@
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>54</v>
       </c>
@@ -2000,7 +2017,7 @@
       </c>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>54</v>
       </c>
@@ -2016,7 +2033,7 @@
       </c>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>54</v>
       </c>
@@ -2032,7 +2049,7 @@
       </c>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>54</v>
       </c>
@@ -2048,7 +2065,7 @@
       </c>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>54</v>
       </c>
@@ -2064,7 +2081,7 @@
       </c>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>54</v>
       </c>
@@ -2080,7 +2097,7 @@
       </c>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>54</v>
       </c>
@@ -2096,7 +2113,7 @@
       </c>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>54</v>
       </c>
@@ -2112,7 +2129,7 @@
       </c>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>54</v>
       </c>
@@ -2128,7 +2145,7 @@
       </c>
       <c r="G73" s="3"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2148,7 +2165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -2168,7 +2185,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>500</v>
       </c>
@@ -2184,23 +2201,38 @@
       <c r="E78" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="18">
         <v>62</v>
       </c>
-      <c r="G78" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I78" s="3" t="s">
+      <c r="G78" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I78" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J78" s="3" t="s">
+      <c r="J78" s="18" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78">
+        <v>38</v>
+      </c>
+      <c r="L78" t="s">
+        <v>90</v>
+      </c>
+      <c r="M78" t="s">
+        <v>91</v>
+      </c>
+      <c r="N78" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O78" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>100</v>
       </c>
@@ -2216,23 +2248,26 @@
       <c r="E79" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="17">
         <v>63</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J79" s="3" t="s">
+      <c r="G79" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H79" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J79" s="17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>100</v>
       </c>
@@ -2248,20 +2283,23 @@
       <c r="E80" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F80" s="3">
+      <c r="F80" s="17">
         <v>64</v>
       </c>
-      <c r="G80" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J80" s="3" t="s">
+      <c r="G80" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H80" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J80" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K80">
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2280,20 +2318,23 @@
       <c r="E81" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="17">
         <v>65</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J81" s="3" t="s">
+      <c r="G81" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H81" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I81" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J81" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K81">
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -2312,27 +2353,30 @@
       <c r="E82" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="17">
         <v>66</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I82" s="3" t="s">
+      <c r="G82" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="J82" s="3" t="s">
+      <c r="J82" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K82">
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C83" s="10"/>
       <c r="D83" s="4"/>
       <c r="G83" s="3"/>
-      <c r="H83" s="2"/>
+      <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="11"/>
     </row>
@@ -2352,20 +2396,23 @@
       <c r="E84" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="17">
         <v>67</v>
       </c>
-      <c r="G84" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J84" s="3" t="s">
+      <c r="G84" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H84" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I84" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J84" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K84">
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -2384,20 +2431,23 @@
       <c r="E85" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="17">
         <v>68</v>
       </c>
-      <c r="G85" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J85" s="3" t="s">
+      <c r="G85" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H85" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I85" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J85" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K85">
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -2416,20 +2466,23 @@
       <c r="E86" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="17">
         <v>69</v>
       </c>
-      <c r="G86" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J86" s="3" t="s">
+      <c r="G86" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I86" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J86" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K86">
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -2448,20 +2501,23 @@
       <c r="E87" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="17">
         <v>70</v>
       </c>
-      <c r="G87" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J87" s="3" t="s">
+      <c r="G87" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I87" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J87" s="17" t="s">
         <v>76</v>
+      </c>
+      <c r="K87">
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -2488,16 +2544,16 @@
       <c r="E89" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F89" s="3">
+      <c r="F89" s="17">
         <v>71</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I89" s="13" t="s">
+      <c r="G89" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H89" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I89" s="19" t="s">
         <v>28</v>
       </c>
       <c r="J89" s="3"/>
@@ -2518,16 +2574,16 @@
       <c r="E90" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="17">
         <v>72</v>
       </c>
-      <c r="G90" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I90" s="3" t="s">
+      <c r="G90" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H90" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I90" s="17" t="s">
         <v>29</v>
       </c>
       <c r="J90" s="3"/>
@@ -2551,13 +2607,13 @@
       <c r="F91" s="17">
         <v>73</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I91" s="3" t="s">
+      <c r="G91" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H91" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I91" s="17" t="s">
         <v>29</v>
       </c>
       <c r="J91" s="3"/>
@@ -2578,22 +2634,22 @@
       <c r="E92" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F92" s="17">
+      <c r="F92" s="18">
         <v>74</v>
       </c>
-      <c r="G92" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H92" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I92" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J92" s="17" t="s">
+      <c r="G92" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H92" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I92" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J92" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="K92" s="17">
+      <c r="K92" s="3">
         <v>50</v>
       </c>
     </row>
@@ -2613,19 +2669,19 @@
       <c r="E93" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="17">
         <v>75</v>
       </c>
-      <c r="G93" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I93" s="3" t="s">
+      <c r="G93" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I93" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K93" s="17">
+      <c r="K93" s="3">
         <v>51</v>
       </c>
     </row>
@@ -2636,7 +2692,7 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-      <c r="K94" s="17"/>
+      <c r="K94" s="3"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
@@ -2654,19 +2710,19 @@
       <c r="E95" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="17">
         <v>76</v>
       </c>
-      <c r="G95" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K95" s="17">
+      <c r="G95" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I95" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K95" s="3">
         <v>52</v>
       </c>
     </row>
@@ -2686,23 +2742,23 @@
       <c r="E96" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="17">
         <v>77</v>
       </c>
-      <c r="G96" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I96" s="3" t="s">
+      <c r="G96" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H96" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I96" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K96" s="17">
+      <c r="K96" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>100</v>
       </c>
@@ -2718,23 +2774,23 @@
       <c r="E97" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="17">
         <v>78</v>
       </c>
-      <c r="G97" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I97" s="3" t="s">
+      <c r="G97" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H97" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I97" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K97" s="17">
+      <c r="K97" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>100</v>
       </c>
@@ -2750,28 +2806,32 @@
       <c r="E98" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F98" s="3">
+      <c r="F98" s="18">
         <v>79</v>
       </c>
-      <c r="G98" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K98" s="17">
+      <c r="G98" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I98" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J98" s="18"/>
+      <c r="K98" s="18">
         <v>55</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E103" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E104" s="3">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
updates MockSample in mock_morphology_generator.py for new input file format
</commit_message>
<xml_diff>
--- a/master_index_key.xlsx
+++ b/master_index_key.xlsx
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E73" workbookViewId="0">
-      <selection activeCell="M85" sqref="M85"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2530,7 @@
       <c r="J89" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K89" s="3">
+      <c r="K89" s="5">
         <v>47</v>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
         <v>28</v>
       </c>
       <c r="J92" s="3"/>
-      <c r="K92" s="3">
+      <c r="K92" s="5">
         <v>50</v>
       </c>
     </row>
@@ -2801,7 +2801,7 @@
       <c r="J98" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K98" s="3">
+      <c r="K98" s="5">
         <v>55</v>
       </c>
     </row>

</xml_diff>